<commit_message>
new table: k1 and k2 range with time
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24423"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\8) term 7\1 mach learn\proj-3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Semester 7\Compution Intelligance\Project\Phase3\KNN-image-classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9679A9-A42C-4409-9A53-7200AE05B60B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8E421D-FC29-4232-9A38-35BD9B8454C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9635B448-68DA-4D5D-9014-199C3BB77A2B}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{9635B448-68DA-4D5D-9014-199C3BB77A2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,33 +20,32 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>k1\k2</t>
   </si>
   <si>
-    <t>Sum</t>
+    <t>time</t>
   </si>
   <si>
-    <t>Average</t>
+    <t>3</t>
   </si>
   <si>
-    <t>Running Total</t>
+    <t>4</t>
   </si>
   <si>
-    <t>Count</t>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
   </si>
 </sst>
 </file>
@@ -57,19 +56,19 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -106,7 +105,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -121,13 +120,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -139,11 +135,187 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="21" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="26" formatCode="h:mm:ss"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="26" formatCode="h:mm:ss"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="26" formatCode="h:mm:ss"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="26" formatCode="h:mm:ss"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="26" formatCode="h:mm:ss"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -159,6 +331,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16625B49-1BB7-4B26-9A10-440B8C699C4E}" name="Table1" displayName="Table1" ref="A21:F31" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A21:F31" xr:uid="{16625B49-1BB7-4B26-9A10-440B8C699C4E}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{2DD16F70-866E-41D8-B491-C79288130479}" name="k1\k2" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{C62E7463-37CC-40D0-B44C-8BA4C967C1EF}" name="3" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{5EED5638-D76B-4888-8483-0F4FFCA192B1}" name="4" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{898BDDA0-6956-418D-823B-3D45025C4A86}" name="5" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{7CFB2D6D-AE2B-48A7-90FB-4284B9A47638}" name="6" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{944581E1-3E71-4324-A65C-9537EDF873E6}" name="7" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -458,21 +645,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C06A6621-AE46-4196-98D9-A594F4355B1A}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="165" zoomScaleNormal="165" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="165" zoomScaleNormal="165" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="8.88671875" style="2"/>
-    <col min="3" max="3" width="8.88671875" style="1"/>
-    <col min="5" max="5" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="8.875" style="2"/>
+    <col min="3" max="3" width="8.875" style="1"/>
+    <col min="5" max="5" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4">
@@ -490,7 +677,7 @@
       <c r="F1" s="4">
         <v>14</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="4">
@@ -509,7 +696,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>3</v>
       </c>
@@ -528,26 +715,26 @@
       <c r="F2" s="3">
         <v>79.251000000000005</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="8">
         <v>5</v>
       </c>
-      <c r="I2" s="10">
+      <c r="I2" s="9">
         <v>83.403999999999996</v>
       </c>
-      <c r="J2" s="10">
+      <c r="J2" s="9">
         <v>83.692999999999998</v>
       </c>
-      <c r="K2" s="10">
+      <c r="K2" s="9">
         <v>83.858999999999995</v>
       </c>
-      <c r="L2" s="10">
+      <c r="L2" s="9">
         <v>83.537000000000006</v>
       </c>
-      <c r="M2" s="10">
+      <c r="M2" s="9">
         <v>83.141999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>4</v>
       </c>
@@ -566,26 +753,26 @@
       <c r="F3" s="5">
         <v>80.521000000000001</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="8">
         <v>6</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="10">
         <v>83.525999999999996</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="10">
         <v>83.936999999999998</v>
       </c>
-      <c r="K3" s="11">
+      <c r="K3" s="10">
         <v>84.128</v>
       </c>
-      <c r="L3" s="11">
+      <c r="L3" s="10">
         <v>83.731999999999999</v>
       </c>
-      <c r="M3" s="11">
+      <c r="M3" s="10">
         <v>83.361000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>5</v>
       </c>
@@ -604,26 +791,26 @@
       <c r="F4" s="3">
         <v>80.959999999999994</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="8">
         <v>7</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="9">
         <v>83.525999999999996</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="9">
         <v>83.912999999999997</v>
       </c>
-      <c r="K4" s="10">
+      <c r="K4" s="9">
         <v>84.152000000000001</v>
       </c>
-      <c r="L4" s="10">
+      <c r="L4" s="9">
         <v>83.951999999999998</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="9">
         <v>83.557000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>6</v>
       </c>
@@ -642,26 +829,26 @@
       <c r="F5" s="5">
         <v>81.058000000000007</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="8">
         <v>8</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="10">
         <v>83.429000000000002</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="10">
         <v>83.936999999999998</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="10">
         <v>84.078999999999994</v>
       </c>
-      <c r="L5" s="11">
+      <c r="L5" s="10">
         <v>83.879000000000005</v>
       </c>
-      <c r="M5" s="11">
+      <c r="M5" s="10">
         <v>83.63</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>7</v>
       </c>
@@ -680,26 +867,26 @@
       <c r="F6" s="3">
         <v>81.131</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="8">
         <v>9</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="9">
         <v>83.477999999999994</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="9">
         <v>84.01</v>
       </c>
-      <c r="K6" s="10">
+      <c r="K6" s="9">
         <v>84.054000000000002</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="9">
         <v>83.903000000000006</v>
       </c>
-      <c r="M6" s="10">
+      <c r="M6" s="9">
         <v>83.703000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>8</v>
       </c>
@@ -718,26 +905,26 @@
       <c r="F7" s="5">
         <v>81.253</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="8">
         <v>10</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="10">
         <v>83.551000000000002</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="10">
         <v>84.058999999999997</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="10">
         <v>84.152000000000001</v>
       </c>
-      <c r="L7" s="11">
+      <c r="L7" s="10">
         <v>83.951999999999998</v>
       </c>
-      <c r="M7" s="11">
+      <c r="M7" s="10">
         <v>83.873999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>9</v>
       </c>
@@ -756,26 +943,26 @@
       <c r="F8" s="3">
         <v>81.350999999999999</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="8">
         <v>11</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="9">
         <v>83.525999999999996</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="9">
         <v>84.108000000000004</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="9">
         <v>84.200999999999993</v>
       </c>
-      <c r="L8" s="10">
+      <c r="L8" s="9">
         <v>83.951999999999998</v>
       </c>
-      <c r="M8" s="10">
+      <c r="M8" s="9">
         <v>83.899000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>10</v>
       </c>
@@ -794,26 +981,26 @@
       <c r="F9" s="5">
         <v>81.448999999999998</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="8">
         <v>12</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="10">
         <v>83.525999999999996</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="10">
         <v>84.132000000000005</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="10">
         <v>84.25</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="10">
         <v>83.951999999999998</v>
       </c>
-      <c r="M9" s="11">
+      <c r="M9" s="10">
         <v>83.923000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>11</v>
       </c>
@@ -832,26 +1019,26 @@
       <c r="F10" s="3">
         <v>81.472999999999999</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="8">
         <v>13</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="9">
         <v>83.501999999999995</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="9">
         <v>84.132000000000005</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="9">
         <v>84.25</v>
       </c>
-      <c r="L10" s="10">
+      <c r="L10" s="9">
         <v>83.977000000000004</v>
       </c>
-      <c r="M10" s="10">
+      <c r="M10" s="9">
         <v>83.923000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>12</v>
       </c>
@@ -870,26 +1057,26 @@
       <c r="F11" s="5">
         <v>81.522000000000006</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="8">
         <v>14</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="10">
         <v>83.477999999999994</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="10">
         <v>84.132000000000005</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="10">
         <v>84.25</v>
       </c>
-      <c r="L11" s="11">
+      <c r="L11" s="10">
         <v>84.025000000000006</v>
       </c>
-      <c r="M11" s="11">
+      <c r="M11" s="10">
         <v>83.923000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>13</v>
       </c>
@@ -909,7 +1096,7 @@
         <v>81.522000000000006</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>14</v>
       </c>
@@ -927,11 +1114,239 @@
       </c>
       <c r="F13" s="6">
         <v>81.497</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="8">
+        <v>5</v>
+      </c>
+      <c r="B22" s="11">
+        <v>1.7361111111111112E-4</v>
+      </c>
+      <c r="C22" s="11">
+        <v>1.9675925925925926E-4</v>
+      </c>
+      <c r="D22" s="11">
+        <v>1.7361111111111112E-4</v>
+      </c>
+      <c r="E22" s="11">
+        <v>1.7361111111111112E-4</v>
+      </c>
+      <c r="F22" s="11">
+        <v>1.6203703703703703E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="8">
+        <v>6</v>
+      </c>
+      <c r="B23" s="12">
+        <v>2.199074074074074E-4</v>
+      </c>
+      <c r="C23" s="12">
+        <v>2.199074074074074E-4</v>
+      </c>
+      <c r="D23" s="12">
+        <v>2.4305555555555552E-4</v>
+      </c>
+      <c r="E23" s="12">
+        <v>2.199074074074074E-4</v>
+      </c>
+      <c r="F23" s="12">
+        <v>2.0833333333333335E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="8">
+        <v>7</v>
+      </c>
+      <c r="B24" s="11">
+        <v>2.3148148148148146E-4</v>
+      </c>
+      <c r="C24" s="11">
+        <v>2.3148148148148146E-4</v>
+      </c>
+      <c r="D24" s="11">
+        <v>2.4305555555555552E-4</v>
+      </c>
+      <c r="E24" s="11">
+        <v>2.3148148148148146E-4</v>
+      </c>
+      <c r="F24" s="11">
+        <v>2.0833333333333335E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="8">
+        <v>8</v>
+      </c>
+      <c r="B25" s="11">
+        <v>2.3148148148148146E-4</v>
+      </c>
+      <c r="C25" s="11">
+        <v>2.5462962962962961E-4</v>
+      </c>
+      <c r="D25" s="11">
+        <v>2.5462962962962961E-4</v>
+      </c>
+      <c r="E25" s="11">
+        <v>2.6620370370370372E-4</v>
+      </c>
+      <c r="F25" s="11">
+        <v>2.6620370370370372E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="8">
+        <v>9</v>
+      </c>
+      <c r="B26" s="11">
+        <v>3.0092592592592595E-4</v>
+      </c>
+      <c r="C26" s="11">
+        <v>2.8935185185185189E-4</v>
+      </c>
+      <c r="D26" s="11">
+        <v>2.8935185185185189E-4</v>
+      </c>
+      <c r="E26" s="11">
+        <v>2.8935185185185189E-4</v>
+      </c>
+      <c r="F26" s="11">
+        <v>2.8935185185185189E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="8">
+        <v>10</v>
+      </c>
+      <c r="B27" s="11">
+        <v>3.2407407407407406E-4</v>
+      </c>
+      <c r="C27" s="11">
+        <v>3.3564814814814812E-4</v>
+      </c>
+      <c r="D27" s="11">
+        <v>2.8935185185185189E-4</v>
+      </c>
+      <c r="E27" s="11">
+        <v>2.8935185185185189E-4</v>
+      </c>
+      <c r="F27" s="11">
+        <v>2.8935185185185189E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="8">
+        <v>11</v>
+      </c>
+      <c r="B28" s="11">
+        <v>3.1250000000000001E-4</v>
+      </c>
+      <c r="C28" s="11">
+        <v>3.1250000000000001E-4</v>
+      </c>
+      <c r="D28" s="11">
+        <v>3.3564814814814812E-4</v>
+      </c>
+      <c r="E28" s="11">
+        <v>3.2407407407407406E-4</v>
+      </c>
+      <c r="F28" s="11">
+        <v>3.3564814814814812E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="8">
+        <v>12</v>
+      </c>
+      <c r="B29" s="11">
+        <v>3.7037037037037035E-4</v>
+      </c>
+      <c r="C29" s="11">
+        <v>3.7037037037037035E-4</v>
+      </c>
+      <c r="D29" s="11">
+        <v>3.5879629629629635E-4</v>
+      </c>
+      <c r="E29" s="11">
+        <v>3.8194444444444446E-4</v>
+      </c>
+      <c r="F29" s="11">
+        <v>3.7037037037037035E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="8">
+        <v>13</v>
+      </c>
+      <c r="B30" s="11">
+        <v>3.9351851851851852E-4</v>
+      </c>
+      <c r="C30" s="11">
+        <v>3.9351851851851852E-4</v>
+      </c>
+      <c r="D30" s="11">
+        <v>3.8194444444444446E-4</v>
+      </c>
+      <c r="E30" s="11">
+        <v>3.8194444444444446E-4</v>
+      </c>
+      <c r="F30" s="11">
+        <v>4.1666666666666669E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="8">
+        <v>14</v>
+      </c>
+      <c r="B31" s="11">
+        <v>4.8611111111111104E-4</v>
+      </c>
+      <c r="C31" s="11">
+        <v>4.2824074074074075E-4</v>
+      </c>
+      <c r="D31" s="11">
+        <v>4.1666666666666669E-4</v>
+      </c>
+      <c r="E31" s="11">
+        <v>4.2824074074074075E-4</v>
+      </c>
+      <c r="F31" s="11">
+        <v>4.5138888888888892E-4</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>